<commit_message>
Started working on RNN, added links to theory and documentation
</commit_message>
<xml_diff>
--- a/myproject/boston.xlsx
+++ b/myproject/boston.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elektaonline-my.sharepoint.com/personal/erik_lagerstroem_elekta_com/Documents/Desktop/git-repo/ML-addin-excel/myproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="622" documentId="8_{2B0D7F5F-2BA1-49B5-BC2C-CE3ED9557C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6CFCA370-6646-484B-A7F3-D636DDAF5B78}"/>
+  <xr:revisionPtr revIDLastSave="719" documentId="8_{2B0D7F5F-2BA1-49B5-BC2C-CE3ED9557C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FB33CC86-2BAD-40EC-89E5-045F25130371}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE496C9-D2E6-42AA-8415-060FDB26DCF2}"/>
   </bookViews>
@@ -509,49 +509,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3.2190350315942502</c:v>
+                  <c:v>10.144515625555652</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.911946713196965</c:v>
+                  <c:v>2.3930217188435243</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.292775343813851</c:v>
+                  <c:v>4.7518807606435471</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.474669215327594</c:v>
+                  <c:v>30.031063931892277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41.562925217954927</c:v>
+                  <c:v>39.607452557003292</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26.703891275830241</c:v>
+                  <c:v>20.244019759214126</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.43002193085980345</c:v>
+                  <c:v>5.4747616653916026E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2299165872404378</c:v>
+                  <c:v>3.1172942415118423</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.66591200654875138</c:v>
+                  <c:v>3.0880275240633637E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.6240850863518403</c:v>
+                  <c:v>2.8465658754996523</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99833672125256556</c:v>
+                  <c:v>5.8827417370770059</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.251884091767129</c:v>
+                  <c:v>0.39489188362145977</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19.351534739048816</c:v>
+                  <c:v>12.780524082383044</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.105255333564855</c:v>
+                  <c:v>3.9305939379883057</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>112.07236236110853</c:v>
+                  <c:v>65.293266257184001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -697,49 +697,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>15.394166946411133</c:v>
+                  <c:v>16.785045623779297</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.668550491333008</c:v>
+                  <c:v>18.553060531616211</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.591764450073242</c:v>
+                  <c:v>19.620119094848633</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18.628486633300781</c:v>
+                  <c:v>19.019939422607422</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.653068542480469</c:v>
+                  <c:v>16.806554794311523</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.532419204711914</c:v>
+                  <c:v>15.200664520263672</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.64423942565918</c:v>
+                  <c:v>18.276601791381836</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.14332389831543</c:v>
+                  <c:v>19.434413909912109</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.683965682983398</c:v>
+                  <c:v>17.675727844238281</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.419902801513672</c:v>
+                  <c:v>18.487176895141602</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.399168014526367</c:v>
+                  <c:v>19.974563598632813</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.100627899169922</c:v>
+                  <c:v>19.971595764160156</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.299037933349609</c:v>
+                  <c:v>20.325014114379883</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.594045639038086</c:v>
+                  <c:v>20.017427444458008</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.486423492431641</c:v>
+                  <c:v>19.980424880981445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,16 +1679,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:X509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2028,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>14.686296242460919</v>
+        <v>16.785045623779297</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -2051,19 +2051,19 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>17.165586979777281</v>
+        <v>18.553060531616211</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21.128468079090371</v>
+        <v>19.620119094848633</v>
       </c>
       <c r="B3">
+        <v>14.686296242460919</v>
+      </c>
+      <c r="C3">
         <f>A1</f>
-        <v>14.686296242460919</v>
-      </c>
-      <c r="C3">
-        <v>15.394166946411133</v>
+        <v>16.785045623779297</v>
       </c>
       <c r="D3">
         <v>13.519576801285428</v>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G3">
         <f>(C3-I495)^2</f>
-        <v>3.2190350315942502</v>
+        <v>10.144515625555652</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -2125,14 +2125,14 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>21.355596289211629</v>
+        <v>19.019939422607422</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B17" si="0">A2</f>
         <v>17.165586979777281</v>
       </c>
       <c r="C4">
-        <v>17.668550491333008</v>
+        <f t="shared" ref="C4:C17" si="0">A2</f>
+        <v>18.553060531616211</v>
       </c>
       <c r="D4">
         <v>15.705767616983223</v>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G17" si="3">(C4-I496)^2</f>
-        <v>5.911946713196965</v>
+        <v>2.3930217188435243</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -2200,14 +2200,14 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>20.109024032557418</v>
+        <v>16.806554794311523</v>
       </c>
       <c r="B5">
+        <v>21.128468079090371</v>
+      </c>
+      <c r="C5">
         <f t="shared" si="0"/>
-        <v>21.128468079090371</v>
-      </c>
-      <c r="C5">
-        <v>18.591764450073242</v>
+        <v>19.620119094848633</v>
       </c>
       <c r="D5">
         <v>20.552375658146843</v>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
-        <v>10.292775343813851</v>
+        <v>4.7518807606435471</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -2275,14 +2275,14 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>17.016325459113396</v>
+        <v>15.200664520263672</v>
       </c>
       <c r="B6">
+        <v>21.355596289211629</v>
+      </c>
+      <c r="C6">
         <f t="shared" si="0"/>
-        <v>21.355596289211629</v>
-      </c>
-      <c r="C6">
-        <v>18.628486633300781</v>
+        <v>19.019939422607422</v>
       </c>
       <c r="D6">
         <v>20.432348102531975</v>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>34.474669215327594</v>
+        <v>30.031063931892277</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -2350,14 +2350,14 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>19.853342405425746</v>
+        <v>18.276601791381836</v>
       </c>
       <c r="B7">
+        <v>20.109024032557418</v>
+      </c>
+      <c r="C7">
         <f t="shared" si="0"/>
-        <v>20.109024032557418</v>
-      </c>
-      <c r="C7">
-        <v>16.653068542480469</v>
+        <v>16.806554794311523</v>
       </c>
       <c r="D7">
         <v>16.5431280507004</v>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>41.562925217954927</v>
+        <v>39.607452557003292</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -2425,14 +2425,14 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>20.983051973187045</v>
+        <v>19.434413909912109</v>
       </c>
       <c r="B8">
+        <v>17.016325459113396</v>
+      </c>
+      <c r="C8">
         <f t="shared" si="0"/>
-        <v>17.016325459113396</v>
-      </c>
-      <c r="C8">
-        <v>14.532419204711914</v>
+        <v>15.200664520263672</v>
       </c>
       <c r="D8">
         <v>13.856875875547022</v>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>26.703891275830241</v>
+        <v>20.244019759214126</v>
       </c>
       <c r="H8" s="1">
         <v>4</v>
@@ -2500,14 +2500,14 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>19.334136110543014</v>
+        <v>17.675727844238281</v>
       </c>
       <c r="B9">
+        <v>19.853342405425746</v>
+      </c>
+      <c r="C9">
         <f t="shared" si="0"/>
-        <v>19.853342405425746</v>
-      </c>
-      <c r="C9">
-        <v>17.64423942565918</v>
+        <v>18.276601791381836</v>
       </c>
       <c r="D9">
         <v>19.087415641720575</v>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>0.43002193085980345</v>
+        <v>5.4747616653916026E-4</v>
       </c>
       <c r="H9" s="1">
         <v>5</v>
@@ -2575,14 +2575,14 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>20.041776596134923</v>
+        <v>18.487176895141602</v>
       </c>
       <c r="B10">
+        <v>20.983051973187045</v>
+      </c>
+      <c r="C10">
         <f t="shared" si="0"/>
-        <v>20.983051973187045</v>
-      </c>
-      <c r="C10">
-        <v>19.14332389831543</v>
+        <v>19.434413909912109</v>
       </c>
       <c r="D10">
         <v>21.264593489815383</v>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>4.2299165872404378</v>
+        <v>3.1172942415118423</v>
       </c>
       <c r="H10" s="1">
         <v>6</v>
@@ -2650,14 +2650,14 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>21.862376115353648</v>
+        <v>19.974563598632813</v>
       </c>
       <c r="B11">
+        <v>19.334136110543014</v>
+      </c>
+      <c r="C11">
         <f t="shared" si="0"/>
-        <v>19.334136110543014</v>
-      </c>
-      <c r="C11">
-        <v>16.683965682983398</v>
+        <v>17.675727844238281</v>
       </c>
       <c r="D11">
         <v>18.430139098506068</v>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>0.66591200654875138</v>
+        <v>3.0880275240633637E-2</v>
       </c>
       <c r="H11" s="1">
         <v>7</v>
@@ -2725,14 +2725,14 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>21.11908846684106</v>
+        <v>19.971595764160156</v>
       </c>
       <c r="B12">
+        <v>20.041776596134923</v>
+      </c>
+      <c r="C12">
         <f t="shared" si="0"/>
-        <v>20.041776596134923</v>
-      </c>
-      <c r="C12">
-        <v>18.419902801513672</v>
+        <v>18.487176895141602</v>
       </c>
       <c r="D12">
         <v>20.489076643951186</v>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>2.6240850863518403</v>
+        <v>2.8465658754996523</v>
       </c>
       <c r="H12" s="1">
         <v>8</v>
@@ -2800,14 +2800,14 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>23.443304408460971</v>
+        <v>20.325014114379883</v>
       </c>
       <c r="B13">
+        <v>21.862376115353648</v>
+      </c>
+      <c r="C13">
         <f t="shared" si="0"/>
-        <v>21.862376115353648</v>
-      </c>
-      <c r="C13">
-        <v>23.399168014526367</v>
+        <v>19.974563598632813</v>
       </c>
       <c r="D13">
         <v>23.813045486209347</v>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>0.99833672125256556</v>
+        <v>5.8827417370770059</v>
       </c>
       <c r="H13" s="1">
         <v>9</v>
@@ -2875,14 +2875,14 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>22.717645147738487</v>
+        <v>20.017427444458008</v>
       </c>
       <c r="B14">
+        <v>21.11908846684106</v>
+      </c>
+      <c r="C14">
         <f t="shared" si="0"/>
-        <v>21.11908846684106</v>
-      </c>
-      <c r="C14">
-        <v>22.100627899169922</v>
+        <v>19.971595764160156</v>
       </c>
       <c r="D14">
         <v>22.719753696069329</v>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>2.251884091767129</v>
+        <v>0.39489188362145977</v>
       </c>
       <c r="H14" s="1">
         <v>10</v>
@@ -2950,14 +2950,14 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>21.09621955518805</v>
+        <v>19.980424880981445</v>
       </c>
       <c r="B15">
+        <v>23.443304408460971</v>
+      </c>
+      <c r="C15">
         <f t="shared" si="0"/>
-        <v>23.443304408460971</v>
-      </c>
-      <c r="C15">
-        <v>28.299037933349609</v>
+        <v>20.325014114379883</v>
       </c>
       <c r="D15">
         <v>28.114800442697632</v>
@@ -2972,7 +2972,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>19.351534739048816</v>
+        <v>12.780524082383044</v>
       </c>
       <c r="H15" s="1">
         <v>11</v>
@@ -3025,11 +3025,11 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16">
+        <v>22.717645147738487</v>
+      </c>
+      <c r="C16">
         <f t="shared" si="0"/>
-        <v>22.717645147738487</v>
-      </c>
-      <c r="C16">
-        <v>26.594045639038086</v>
+        <v>20.017427444458008</v>
       </c>
       <c r="D16">
         <v>26.592682525314746</v>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>21.105255333564855</v>
+        <v>3.9305939379883057</v>
       </c>
       <c r="H16" s="1">
         <v>12</v>
@@ -3097,11 +3097,11 @@
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17">
+        <v>21.09621955518805</v>
+      </c>
+      <c r="C17">
         <f t="shared" si="0"/>
-        <v>21.09621955518805</v>
-      </c>
-      <c r="C17">
-        <v>22.486423492431641</v>
+        <v>19.980424880981445</v>
       </c>
       <c r="D17">
         <v>22.741997713588752</v>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>112.07236236110853</v>
+        <v>65.293266257184001</v>
       </c>
       <c r="H17" s="1">
         <v>13</v>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="G18">
         <f>AVERAGE(G3:G17)</f>
-        <v>19.059636777030708</v>
+        <v>13.429950674654995</v>
       </c>
       <c r="H18" s="1">
         <v>14</v>

</xml_diff>

<commit_message>
Further developments and error handling
</commit_message>
<xml_diff>
--- a/myproject/boston.xlsx
+++ b/myproject/boston.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elektaonline-my.sharepoint.com/personal/erik_lagerstroem_elekta_com/Documents/Desktop/git-repo/ML-addin-excel/myproject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="719" documentId="8_{2B0D7F5F-2BA1-49B5-BC2C-CE3ED9557C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FB33CC86-2BAD-40EC-89E5-045F25130371}"/>
+  <xr:revisionPtr revIDLastSave="1097" documentId="8_{2B0D7F5F-2BA1-49B5-BC2C-CE3ED9557C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAF541F5-29AE-446B-8F8D-2FF39AFF74E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4DE496C9-D2E6-42AA-8415-060FDB26DCF2}"/>
   </bookViews>
@@ -295,49 +295,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1.1800395263847132</c:v>
+                  <c:v>2.7665618491607202</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.610779773252629</c:v>
+                  <c:v>7.4427503431992754</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45095512080057665</c:v>
+                  <c:v>0.20943556084533588</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.8872746964196772</c:v>
+                  <c:v>8.7500079829803816</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9459372378190984</c:v>
+                  <c:v>5.1938023396577604</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.2021090414029194</c:v>
+                  <c:v>2.0757596527895279</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4128726284938402</c:v>
+                  <c:v>4.1200443576997952</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.706644633803421E-2</c:v>
+                  <c:v>1.4545590606412518E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.3640552719978545</c:v>
+                  <c:v>5.7284661365523615</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.509115499248125</c:v>
+                  <c:v>12.075266742357465</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.28903944134223269</c:v>
+                  <c:v>0.5097156968809774</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.26945283640740042</c:v>
+                  <c:v>0.33937517079631146</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20857086333118213</c:v>
+                  <c:v>1.9767773488615008</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.51501455807259533</c:v>
+                  <c:v>4.8461464444451005E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84.570454107223085</c:v>
+                  <c:v>86.357759865386811</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -509,49 +509,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>10.144515625555652</c:v>
+                  <c:v>6.7658569809887581</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3930217188435243</c:v>
+                  <c:v>0.80385797068535136</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.7518807606435471</c:v>
+                  <c:v>6.2870802870229854</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.031063931892277</c:v>
+                  <c:v>28.972699198871851</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.607452557003292</c:v>
+                  <c:v>44.674397762509926</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.244019759214126</c:v>
+                  <c:v>25.738068845898518</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.4747616653916026E-4</c:v>
+                  <c:v>2.8438209104936175E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.1172942415118423</c:v>
+                  <c:v>2.4463296891748882</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0880275240633637E-2</c:v>
+                  <c:v>2.2863051017338876E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8465658754996523</c:v>
+                  <c:v>4.9518201404809918</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8827417370770059</c:v>
+                  <c:v>0.26377806983015178</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.39489188362145977</c:v>
+                  <c:v>2.8002270937716776</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.780524082383044</c:v>
+                  <c:v>35.415329760178594</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.9305939379883057</c:v>
+                  <c:v>31.820351469854359</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>65.293266257184001</c:v>
+                  <c:v>122.07802754013115</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -610,49 +610,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>14.686296242460919</c:v>
+                  <c:v>15.263298484686594</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.165586979777281</c:v>
+                  <c:v>17.371859544818253</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.128468079090371</c:v>
+                  <c:v>21.342358698492657</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.355596289211629</c:v>
+                  <c:v>21.541958759080533</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.109024032557418</c:v>
+                  <c:v>20.82100848188113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.016325459113396</c:v>
+                  <c:v>18.259250315707295</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19.853342405425746</c:v>
+                  <c:v>20.329789239724114</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.983051973187045</c:v>
+                  <c:v>21.07939489809128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.334136110543014</c:v>
+                  <c:v>19.893421428949019</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.041776596134923</c:v>
+                  <c:v>20.274948451755431</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.862376115353648</c:v>
+                  <c:v>21.686056236891883</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21.11908846684106</c:v>
+                  <c:v>21.182559156477961</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.443304408460971</c:v>
+                  <c:v>22.49402085760083</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.717645147738487</c:v>
+                  <c:v>22.069614268971563</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.09621955518805</c:v>
+                  <c:v>21.192887595650063</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -697,49 +697,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>16.785045623779297</c:v>
+                  <c:v>16.201126098632813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18.553060531616211</c:v>
+                  <c:v>19.203418731689453</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19.620119094848633</c:v>
+                  <c:v>19.292594909667969</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.019939422607422</c:v>
+                  <c:v>19.11737060546875</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.806554794311523</c:v>
+                  <c:v>16.416109085083008</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.200664520263672</c:v>
+                  <c:v>14.626729965209961</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.276601791381836</c:v>
+                  <c:v>18.283136367797852</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19.434413909912109</c:v>
+                  <c:v>19.63592529296875</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>17.675727844238281</c:v>
+                  <c:v>17.452184677124023</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.487176895141602</c:v>
+                  <c:v>19.0252685546875</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.974563598632813</c:v>
+                  <c:v>22.913593292236328</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.971595764160156</c:v>
+                  <c:v>22.273387908935547</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.325014114379883</c:v>
+                  <c:v>29.851078033447266</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.017427444458008</c:v>
+                  <c:v>27.640953063964844</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19.980424880981445</c:v>
+                  <c:v>22.948892593383789</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2017,7 +2017,7 @@
   <dimension ref="A1:X509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2028,7 +2028,7 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>16.785045623779297</v>
+        <v>15.263298484686594</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -2051,26 +2051,26 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>18.553060531616211</v>
+        <v>17.371859544818253</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>19.620119094848633</v>
+        <v>21.342358698492657</v>
       </c>
       <c r="B3">
-        <v>14.686296242460919</v>
+        <f>A1</f>
+        <v>15.263298484686594</v>
       </c>
       <c r="C3">
-        <f>A1</f>
-        <v>16.785045623779297</v>
+        <v>16.201126098632813</v>
       </c>
       <c r="D3">
         <v>13.519576801285428</v>
       </c>
       <c r="E3">
         <f>(B3-I495)^2</f>
-        <v>1.1800395263847132</v>
+        <v>2.7665618491607202</v>
       </c>
       <c r="F3">
         <f>(D3-I495)^2</f>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G3">
         <f>(C3-I495)^2</f>
-        <v>10.144515625555652</v>
+        <v>6.7658569809887581</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -2125,21 +2125,21 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>19.019939422607422</v>
+        <v>21.541958759080533</v>
       </c>
       <c r="B4">
-        <v>17.165586979777281</v>
+        <f t="shared" ref="B4:B17" si="0">A2</f>
+        <v>17.371859544818253</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C17" si="0">A2</f>
-        <v>18.553060531616211</v>
+        <v>19.203418731689453</v>
       </c>
       <c r="D4">
         <v>15.705767616983223</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E17" si="1">(B4-I496)^2</f>
-        <v>8.610779773252629</v>
+        <v>7.4427503431992754</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F17" si="2">(D4-I496)^2</f>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="G4">
         <f t="shared" ref="G4:G17" si="3">(C4-I496)^2</f>
-        <v>2.3930217188435243</v>
+        <v>0.80385797068535136</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -2200,21 +2200,21 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>16.806554794311523</v>
+        <v>20.82100848188113</v>
       </c>
       <c r="B5">
-        <v>21.128468079090371</v>
+        <f t="shared" si="0"/>
+        <v>21.342358698492657</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>19.620119094848633</v>
+        <v>19.292594909667969</v>
       </c>
       <c r="D5">
         <v>20.552375658146843</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0.45095512080057665</v>
+        <v>0.20943556084533588</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="G5">
         <f t="shared" si="3"/>
-        <v>4.7518807606435471</v>
+        <v>6.2870802870229854</v>
       </c>
       <c r="H5" s="1">
         <v>1</v>
@@ -2275,21 +2275,21 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15.200664520263672</v>
+        <v>18.259250315707295</v>
       </c>
       <c r="B6">
-        <v>21.355596289211629</v>
+        <f t="shared" si="0"/>
+        <v>21.541958759080533</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>19.019939422607422</v>
+        <v>19.11737060546875</v>
       </c>
       <c r="D6">
         <v>20.432348102531975</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>9.8872746964196772</v>
+        <v>8.7500079829803816</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
@@ -2297,7 +2297,7 @@
       </c>
       <c r="G6">
         <f t="shared" si="3"/>
-        <v>30.031063931892277</v>
+        <v>28.972699198871851</v>
       </c>
       <c r="H6" s="1">
         <v>2</v>
@@ -2350,21 +2350,21 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>18.276601791381836</v>
+        <v>20.329789239724114</v>
       </c>
       <c r="B7">
-        <v>20.109024032557418</v>
+        <f t="shared" si="0"/>
+        <v>20.82100848188113</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>16.806554794311523</v>
+        <v>16.416109085083008</v>
       </c>
       <c r="D7">
         <v>16.5431280507004</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>8.9459372378190984</v>
+        <v>5.1938023396577604</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
@@ -2372,7 +2372,7 @@
       </c>
       <c r="G7">
         <f t="shared" si="3"/>
-        <v>39.607452557003292</v>
+        <v>44.674397762509926</v>
       </c>
       <c r="H7" s="1">
         <v>3</v>
@@ -2425,21 +2425,21 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>19.434413909912109</v>
+        <v>21.07939489809128</v>
       </c>
       <c r="B8">
-        <v>17.016325459113396</v>
+        <f t="shared" si="0"/>
+        <v>18.259250315707295</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>15.200664520263672</v>
+        <v>14.626729965209961</v>
       </c>
       <c r="D8">
         <v>13.856875875547022</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>7.2021090414029194</v>
+        <v>2.0757596527895279</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
@@ -2447,7 +2447,7 @@
       </c>
       <c r="G8">
         <f t="shared" si="3"/>
-        <v>20.244019759214126</v>
+        <v>25.738068845898518</v>
       </c>
       <c r="H8" s="1">
         <v>4</v>
@@ -2500,21 +2500,21 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>17.675727844238281</v>
+        <v>19.893421428949019</v>
       </c>
       <c r="B9">
-        <v>19.853342405425746</v>
+        <f t="shared" si="0"/>
+        <v>20.329789239724114</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>18.276601791381836</v>
+        <v>18.283136367797852</v>
       </c>
       <c r="D9">
         <v>19.087415641720575</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>2.4128726284938402</v>
+        <v>4.1200443576997952</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="G9">
         <f t="shared" si="3"/>
-        <v>5.4747616653916026E-4</v>
+        <v>2.8438209104936175E-4</v>
       </c>
       <c r="H9" s="1">
         <v>5</v>
@@ -2575,21 +2575,21 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>18.487176895141602</v>
+        <v>20.274948451755431</v>
       </c>
       <c r="B10">
-        <v>20.983051973187045</v>
+        <f t="shared" si="0"/>
+        <v>21.07939489809128</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>19.434413909912109</v>
+        <v>19.63592529296875</v>
       </c>
       <c r="D10">
         <v>21.264593489815383</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>4.706644633803421E-2</v>
+        <v>1.4545590606412518E-2</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
@@ -2597,7 +2597,7 @@
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>3.1172942415118423</v>
+        <v>2.4463296891748882</v>
       </c>
       <c r="H10" s="1">
         <v>6</v>
@@ -2650,21 +2650,21 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>19.974563598632813</v>
+        <v>21.686056236891883</v>
       </c>
       <c r="B11">
-        <v>19.334136110543014</v>
+        <f t="shared" si="0"/>
+        <v>19.893421428949019</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>17.675727844238281</v>
+        <v>17.452184677124023</v>
       </c>
       <c r="D11">
         <v>18.430139098506068</v>
       </c>
       <c r="E11">
         <f t="shared" si="1"/>
-        <v>3.3640552719978545</v>
+        <v>5.7284661365523615</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
@@ -2672,7 +2672,7 @@
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>3.0880275240633637E-2</v>
+        <v>2.2863051017338876E-3</v>
       </c>
       <c r="H11" s="1">
         <v>7</v>
@@ -2725,21 +2725,21 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>19.971595764160156</v>
+        <v>21.182559156477961</v>
       </c>
       <c r="B12">
-        <v>20.041776596134923</v>
+        <f t="shared" si="0"/>
+        <v>20.274948451755431</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
-        <v>18.487176895141602</v>
+        <v>19.0252685546875</v>
       </c>
       <c r="D12">
         <v>20.489076643951186</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>10.509115499248125</v>
+        <v>12.075266742357465</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>2.8465658754996523</v>
+        <v>4.9518201404809918</v>
       </c>
       <c r="H12" s="1">
         <v>8</v>
@@ -2800,21 +2800,21 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>20.325014114379883</v>
+        <v>22.49402085760083</v>
       </c>
       <c r="B13">
-        <v>21.862376115353648</v>
+        <f t="shared" si="0"/>
+        <v>21.686056236891883</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
-        <v>19.974563598632813</v>
+        <v>22.913593292236328</v>
       </c>
       <c r="D13">
         <v>23.813045486209347</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>0.28903944134223269</v>
+        <v>0.5097156968809774</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>5.8827417370770059</v>
+        <v>0.26377806983015178</v>
       </c>
       <c r="H13" s="1">
         <v>9</v>
@@ -2875,21 +2875,21 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>20.017427444458008</v>
+        <v>22.069614268971563</v>
       </c>
       <c r="B14">
-        <v>21.11908846684106</v>
+        <f t="shared" si="0"/>
+        <v>21.182559156477961</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
-        <v>19.971595764160156</v>
+        <v>22.273387908935547</v>
       </c>
       <c r="D14">
         <v>22.719753696069329</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
-        <v>0.26945283640740042</v>
+        <v>0.33937517079631146</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
@@ -2897,7 +2897,7 @@
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>0.39489188362145977</v>
+        <v>2.8002270937716776</v>
       </c>
       <c r="H14" s="1">
         <v>10</v>
@@ -2950,21 +2950,21 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>19.980424880981445</v>
+        <v>21.192887595650063</v>
       </c>
       <c r="B15">
-        <v>23.443304408460971</v>
+        <f t="shared" si="0"/>
+        <v>22.49402085760083</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>20.325014114379883</v>
+        <v>29.851078033447266</v>
       </c>
       <c r="D15">
         <v>28.114800442697632</v>
       </c>
       <c r="E15">
         <f t="shared" si="1"/>
-        <v>0.20857086333118213</v>
+        <v>1.9767773488615008</v>
       </c>
       <c r="F15">
         <f t="shared" si="2"/>
@@ -2972,7 +2972,7 @@
       </c>
       <c r="G15">
         <f t="shared" si="3"/>
-        <v>12.780524082383044</v>
+        <v>35.415329760178594</v>
       </c>
       <c r="H15" s="1">
         <v>11</v>
@@ -3025,18 +3025,18 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>22.717645147738487</v>
+        <f t="shared" si="0"/>
+        <v>22.069614268971563</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
-        <v>20.017427444458008</v>
+        <v>27.640953063964844</v>
       </c>
       <c r="D16">
         <v>26.592682525314746</v>
       </c>
       <c r="E16">
         <f t="shared" si="1"/>
-        <v>0.51501455807259533</v>
+        <v>4.8461464444451005E-3</v>
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
@@ -3044,7 +3044,7 @@
       </c>
       <c r="G16">
         <f t="shared" si="3"/>
-        <v>3.9305939379883057</v>
+        <v>31.820351469854359</v>
       </c>
       <c r="H16" s="1">
         <v>12</v>
@@ -3097,18 +3097,18 @@
     </row>
     <row r="17" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B17">
-        <v>21.09621955518805</v>
+        <f t="shared" si="0"/>
+        <v>21.192887595650063</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
-        <v>19.980424880981445</v>
+        <v>22.948892593383789</v>
       </c>
       <c r="D17">
         <v>22.741997713588752</v>
       </c>
       <c r="E17">
         <f t="shared" si="1"/>
-        <v>84.570454107223085</v>
+        <v>86.357759865386811</v>
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="G17">
         <f t="shared" si="3"/>
-        <v>65.293266257184001</v>
+        <v>122.07802754013115</v>
       </c>
       <c r="H17" s="1">
         <v>13</v>
@@ -3170,7 +3170,7 @@
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E18">
         <f>AVERAGE(E3:E17)</f>
-        <v>9.2308491365689314</v>
+        <v>9.171007652281272</v>
       </c>
       <c r="F18">
         <f>AVERAGE(F3:F17)</f>
@@ -3178,7 +3178,7 @@
       </c>
       <c r="G18">
         <f>AVERAGE(G3:G17)</f>
-        <v>13.429950674654995</v>
+        <v>20.868026366439462</v>
       </c>
       <c r="H18" s="1">
         <v>14</v>

</xml_diff>